<commit_message>
modified excel sheet and data provider class
</commit_message>
<xml_diff>
--- a/Datasheet/iManage_data.xlsx
+++ b/Datasheet/iManage_data.xlsx
@@ -4,55 +4,27 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="12105" windowHeight="10245" tabRatio="675" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="12105" windowHeight="10245" tabRatio="886" activeTab="8"/>
   </bookViews>
   <sheets>
-    <sheet name="Invoice" sheetId="1" r:id="rId1"/>
-    <sheet name="Configuration" sheetId="24" r:id="rId2"/>
-    <sheet name="Login" sheetId="2" r:id="rId3"/>
-    <sheet name="MyTemplates" sheetId="14" r:id="rId4"/>
-    <sheet name="NewBatch" sheetId="19" r:id="rId5"/>
-    <sheet name="ProcessForm" sheetId="20" r:id="rId6"/>
+    <sheet name="Login" sheetId="2" r:id="rId1"/>
+    <sheet name="MyTemplates" sheetId="14" r:id="rId2"/>
+    <sheet name="StandardDashboard" sheetId="25" r:id="rId3"/>
+    <sheet name="CustomDashboard" sheetId="26" r:id="rId4"/>
+    <sheet name="WorkbenchTrack" sheetId="28" r:id="rId5"/>
+    <sheet name="WorkbenchReview" sheetId="30" r:id="rId6"/>
+    <sheet name="WorkbenchApproval" sheetId="31" r:id="rId7"/>
+    <sheet name="WorkbenchMyTasks" sheetId="29" r:id="rId8"/>
+    <sheet name="MyReports" sheetId="27" r:id="rId9"/>
+    <sheet name="NewBatch" sheetId="19" r:id="rId10"/>
+    <sheet name="ProcessForm" sheetId="20" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="110">
-  <si>
-    <t>invoice_name</t>
-  </si>
-  <si>
-    <t>invoice_status</t>
-  </si>
-  <si>
-    <t>Submitted</t>
-  </si>
-  <si>
-    <t>doc_type</t>
-  </si>
-  <si>
-    <t>Invoice</t>
-  </si>
-  <si>
-    <t>invoiceno</t>
-  </si>
-  <si>
-    <t>location</t>
-  </si>
-  <si>
-    <t>currency</t>
-  </si>
-  <si>
-    <t>paymentterm</t>
-  </si>
-  <si>
-    <t>INR</t>
-  </si>
-  <si>
-    <t>Net12</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="88">
   <si>
     <t>flag</t>
   </si>
@@ -78,48 +50,6 @@
     <t>ZCS</t>
   </si>
   <si>
-    <t>hinal</t>
-  </si>
-  <si>
-    <t>Indiana (IDD)</t>
-  </si>
-  <si>
-    <t>supplier_company</t>
-  </si>
-  <si>
-    <t>GDQA_SUPPLIER</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>item_no</t>
-  </si>
-  <si>
-    <t>item_description</t>
-  </si>
-  <si>
-    <t>product_category</t>
-  </si>
-  <si>
-    <t>market_price</t>
-  </si>
-  <si>
-    <t>test_item</t>
-  </si>
-  <si>
-    <t>Materials testing</t>
-  </si>
-  <si>
-    <t>quantity</t>
-  </si>
-  <si>
-    <t>credit_memoNo</t>
-  </si>
-  <si>
-    <t>test_item1</t>
-  </si>
-  <si>
     <t>Amerihealth</t>
   </si>
   <si>
@@ -324,24 +254,6 @@
     <t>AXA Equitable Life Insurance</t>
   </si>
   <si>
-    <t>Browser</t>
-  </si>
-  <si>
-    <t>Chrome</t>
-  </si>
-  <si>
-    <t>Environment</t>
-  </si>
-  <si>
-    <t>Partner</t>
-  </si>
-  <si>
-    <t>Staging</t>
-  </si>
-  <si>
-    <t>iContract</t>
-  </si>
-  <si>
     <t>ZCS Production</t>
   </si>
   <si>
@@ -349,6 +261,33 @@
   </si>
   <si>
     <t>My Templates</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>Standard Dashboard</t>
+  </si>
+  <si>
+    <t>Custom Dashboard</t>
+  </si>
+  <si>
+    <t>My Reports</t>
+  </si>
+  <si>
+    <t>Workbench</t>
+  </si>
+  <si>
+    <t>Track</t>
+  </si>
+  <si>
+    <t>My Tasks</t>
+  </si>
+  <si>
+    <t>Review</t>
+  </si>
+  <si>
+    <t>Approval</t>
   </si>
 </sst>
 </file>
@@ -698,233 +637,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N1" t="s">
-        <v>30</v>
-      </c>
-      <c r="O1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2">
-        <v>5743897</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2">
-        <v>1357</v>
-      </c>
-      <c r="K2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2">
-        <v>1000</v>
-      </c>
-      <c r="N2">
-        <v>60</v>
-      </c>
-      <c r="O2">
-        <v>885390</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3">
-        <v>73429</v>
-      </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3">
-        <v>1357</v>
-      </c>
-      <c r="K3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3">
-        <v>1000</v>
-      </c>
-      <c r="N3">
-        <v>60</v>
-      </c>
-      <c r="O3">
-        <v>906840</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -942,242 +654,242 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="E5" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="E6" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="E7" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="E8" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="C9" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="E9" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="C10" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="E10" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="C11" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="E11" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>98</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>108</v>
-      </c>
-      <c r="C12" t="s">
-        <v>83</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E12" t="s">
-        <v>107</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1213,46 +925,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection sqref="A1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1264,54 +942,54 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="F1" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="G1" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="H1" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="G2" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="H2" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1319,7 +997,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T2"/>
   <sheetViews>
@@ -1350,105 +1028,105 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="E1" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="F1" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="G1" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="H1" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="I1" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="J1" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="K1" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="L1" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="M1" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="N1" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="O1" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="P1" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="Q1" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="R1" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="S1" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="T1" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="F2" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="G2" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="H2" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="I2" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="J2" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="K2" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="L2" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="M2" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="N2">
         <v>6</v>
@@ -1466,10 +1144,313 @@
         <v>1</v>
       </c>
       <c r="S2" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="T2" t="s">
-        <v>53</v>
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>